<commit_message>
Overwrite with local folder
</commit_message>
<xml_diff>
--- a/appointments.xlsx
+++ b/appointments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,6 +975,158 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mona</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0555935549</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Polestar 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>test drive</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>عبدالله محمد عبدالرحيم</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>65444356694</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>76905</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>تايوتا هايليندر مودل عام ٢٠٢٣</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-01</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>عبدالله محمد عبدالرهيب</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0500556694</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>76905</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>تيوتا هايلندر 2023</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1-5-2025</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mona</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0555935549</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Polestar 2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>test drive</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mohammed Al-Naim</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Dodge RAM 1500 Limited</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>